<commit_message>
calorimetry : scripts : more metrics
</commit_message>
<xml_diff>
--- a/output/calorimetry/ds.10.ampoule.no.opt/data.xlsx
+++ b/output/calorimetry/ds.10.ampoule.no.opt/data.xlsx
@@ -9,7 +9,7 @@
     <sheet name="equilibrium_concentrations" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="heats_calculated" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="enthalpies_calculated" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="adj_r_squared" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="metrics" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="input_stoich_coefficients" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="input_concentrations" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="input_k_constants_log10" sheetId="7" state="visible" r:id="rId7"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">M</t>
   </si>
@@ -119,9 +119,39 @@
     <t xml:space="preserve">dev</t>
   </si>
   <si>
+    <t xml:space="preserve">metrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj.R^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRMSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMAPE</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3</t>
+  </si>
+  <si>
     <t xml:space="preserve">tot</t>
   </si>
   <si>
@@ -171,9 +201,6 @@
   </si>
   <si>
     <t xml:space="preserve">initial volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
@@ -1054,15 +1081,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1070,16 +1097,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1459,8 +1486,35 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="n">
         <v>0.999953533181825</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.00111954606999985</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.000792263715949105</v>
       </c>
     </row>
   </sheetData>
@@ -1491,157 +1545,157 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-1</v>
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>0</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -1663,19 +1717,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2">
@@ -1697,16 +1751,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -1714,16 +1768,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -1731,16 +1785,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1748,16 +1802,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -1765,16 +1819,16 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -1782,16 +1836,16 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
         <v>25</v>
@@ -1799,16 +1853,16 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
@@ -1816,16 +1870,16 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
         <v>26</v>
@@ -1833,16 +1887,16 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
         <v>28</v>
@@ -1850,16 +1904,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
@@ -1867,36 +1921,36 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1915,7 +1969,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">

</xml_diff>